<commit_message>
Flex PCB finished. Need to rotate RFID transponder coil.
</commit_message>
<xml_diff>
--- a/Documentation/BOMs/RFID Module BOM.xlsx
+++ b/Documentation/BOMs/RFID Module BOM.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bens1\Documents\Other\Projects\Smart-Watch\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bens1\Documents\Other\Projects\Smart-Watch\Documentation\BOMs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5917E8C0-26C2-416A-BC3B-9738E6ACADDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{287DB8CE-41AD-48A1-9C7A-B197A4A90B32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{2CD4C552-014C-46CB-A006-06574E6AD0D8}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>TLV9004SIRTER</t>
   </si>
@@ -114,6 +114,9 @@
   </si>
   <si>
     <t>Inductors</t>
+  </si>
+  <si>
+    <t>Alternative: 4513TC-495XGLB</t>
   </si>
 </sst>
 </file>
@@ -480,24 +483,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2854E2AE-1F84-4BA7-92E0-89D110801EEE}">
-  <dimension ref="A3:I12"/>
+  <dimension ref="A3:J12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="12.77734375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C4" t="s">
         <v>0</v>
       </c>
@@ -515,7 +519,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C5" t="s">
         <v>3</v>
       </c>
@@ -533,7 +537,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -557,7 +561,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C8" t="s">
         <v>10</v>
       </c>
@@ -575,7 +579,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
         <v>14</v>
       </c>
@@ -596,7 +600,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>24</v>
       </c>
@@ -623,6 +627,9 @@
       </c>
       <c r="I12" s="3" t="s">
         <v>23</v>
+      </c>
+      <c r="J12" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>